<commit_message>
Adds more chapter 10 digit code files
</commit_message>
<xml_diff>
--- a/public/cn2021_2022/2022 10 digit codes Chapter 08.xlsx
+++ b/public/cn2021_2022/2022 10 digit codes Chapter 08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc-my.sharepoint.com/personal/david_harris2_hmrc_gov_uk/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{96E1156C-23C6-4789-927C-933E11A68600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{94F61929-AB08-49A3-A889-A15A7CA62849}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{96E1156C-23C6-4789-927C-933E11A68600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DE1B4FB7-5F54-402C-A4E1-DF5B3275826F}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{564801B8-4F29-452E-BCB1-90E08E7A622D}"/>
+    <workbookView minimized="1" xWindow="1778" yWindow="1778" windowWidth="15390" windowHeight="9532" xr2:uid="{564801B8-4F29-452E-BCB1-90E08E7A622D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>10 Digit Codes Deleted from 1 January 2022</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t xml:space="preserve">Pine nuts, shelled </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 0811 9050 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 0811 9050 90</t>
+  </si>
+  <si>
+    <t>Fruit of the genus Vaccinium, uncooked or cooked by steaming or boiling in water, frozen, not containing added sugar or other sweetening matter</t>
   </si>
 </sst>
 </file>
@@ -139,10 +148,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -161,7 +179,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -181,6 +199,15 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -506,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0328BFC-B905-4C6A-A5B7-256E46A41FD3}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -555,37 +582,62 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>13</v>
+    <row r="7" spans="1:2" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>